<commit_message>
penilaian kelas XII RPL 3 pertemuan 1
</commit_message>
<xml_diff>
--- a/XIIRPL3(✿◕‿◕✿)(✿◕‿◕✿)(✿◕‿◕✿)/DATA PRAKTIK XII RPl 3.xlsx
+++ b/XIIRPL3(✿◕‿◕✿)(✿◕‿◕✿)(✿◕‿◕✿)/DATA PRAKTIK XII RPl 3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00. Ade Setiyawan (berkas penting pribadi)\SMKN1 JATIROTO\MAPEL PWPB XII\pwpb2223\XIIRPL3(✿◕‿◕✿)(✿◕‿◕✿)(✿◕‿◕✿)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL3(✿◕‿◕✿)(✿◕‿◕✿)(✿◕‿◕✿)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EEBF14-99F7-47F1-A04F-48C1FE28981B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20CD5D0-7892-444E-B776-C47CE278E745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$D$38</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">Nama </t>
   </si>
@@ -102,6 +110,114 @@
   <si>
     <t>ULANGAN
 1</t>
+  </si>
+  <si>
+    <t>Agus</t>
+  </si>
+  <si>
+    <t>Ahmad</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>Aldi</t>
+  </si>
+  <si>
+    <t>Amelia</t>
+  </si>
+  <si>
+    <t>Andila</t>
+  </si>
+  <si>
+    <t>Aulia</t>
+  </si>
+  <si>
+    <t>Elfira</t>
+  </si>
+  <si>
+    <t>Erlangga</t>
+  </si>
+  <si>
+    <t>Ervina</t>
+  </si>
+  <si>
+    <t>Evelyn</t>
+  </si>
+  <si>
+    <t>Febriyan</t>
+  </si>
+  <si>
+    <t>Felandini</t>
+  </si>
+  <si>
+    <t>Ferdian</t>
+  </si>
+  <si>
+    <t>Fitri</t>
+  </si>
+  <si>
+    <t>Gilang</t>
+  </si>
+  <si>
+    <t>Gama</t>
+  </si>
+  <si>
+    <t>Nisa</t>
+  </si>
+  <si>
+    <t>Yani</t>
+  </si>
+  <si>
+    <t>Lina</t>
+  </si>
+  <si>
+    <t>Melycha</t>
+  </si>
+  <si>
+    <t>Robby</t>
+  </si>
+  <si>
+    <t>Cello</t>
+  </si>
+  <si>
+    <t>Nabila</t>
+  </si>
+  <si>
+    <t>Novi</t>
+  </si>
+  <si>
+    <t>Bekti</t>
+  </si>
+  <si>
+    <t>Nurma</t>
+  </si>
+  <si>
+    <t>Panji</t>
+  </si>
+  <si>
+    <t>Praditha</t>
+  </si>
+  <si>
+    <t>Rena</t>
+  </si>
+  <si>
+    <t>Siti</t>
+  </si>
+  <si>
+    <t>Sopyan</t>
+  </si>
+  <si>
+    <t>Tiyas</t>
+  </si>
+  <si>
+    <t>Warseno</t>
+  </si>
+  <si>
+    <t>Windhi</t>
+  </si>
+  <si>
+    <t>Yusroofa</t>
   </si>
 </sst>
 </file>
@@ -455,6 +571,24 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -476,15 +610,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -493,15 +618,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -825,16 +941,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" style="2" customWidth="1"/>
     <col min="4" max="6" width="12.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
@@ -844,43 +960,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="A1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="23" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="18" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="29"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="15" t="s">
         <v>10</v>
       </c>
@@ -908,41 +1024,47 @@
       <c r="M2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="19"/>
-      <c r="O2" s="18"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="13"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="18"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="C4" s="6">
         <f t="shared" ref="C4:C38" si="0">((SUM(D4:M4)*10)*70%)+(AVERAGE(N4:O4)*30%)</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -962,12 +1084,16 @@
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -988,12 +1114,16 @@
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -1014,13 +1144,19 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -1040,12 +1176,16 @@
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="C8" s="6">
         <f>((SUM(D8:M8)*10)*70%)+(AVERAGE(N8:O8)*30%)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -1066,13 +1206,19 @@
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10"/>
+        <v>12.25</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.75</v>
+      </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -1092,13 +1238,19 @@
       <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -1118,12 +1270,16 @@
       <c r="A11" s="3">
         <v>8</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -1144,13 +1300,19 @@
       <c r="A12" s="3">
         <v>9</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1170,12 +1332,16 @@
       <c r="A13" s="3">
         <v>10</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1196,12 +1362,16 @@
       <c r="A14" s="3">
         <v>11</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D14" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -1222,12 +1392,16 @@
       <c r="A15" s="3">
         <v>12</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D15" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -1248,12 +1422,16 @@
       <c r="A16" s="3">
         <v>13</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D16" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -1274,13 +1452,19 @@
       <c r="A17" s="3">
         <v>14</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+        <v>12.25</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.75</v>
+      </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1300,12 +1484,16 @@
       <c r="A18" s="3">
         <v>15</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -1326,13 +1514,19 @@
       <c r="A19" s="3">
         <v>16</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+        <v>12.25</v>
+      </c>
+      <c r="D19" s="10">
+        <v>1</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.75</v>
+      </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -1352,12 +1546,16 @@
       <c r="A20" s="3">
         <v>17</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D20" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="D20" s="11">
+        <v>1</v>
+      </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -1378,13 +1576,19 @@
       <c r="A21" s="3">
         <v>18</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
@@ -1404,12 +1608,16 @@
       <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -1430,13 +1638,19 @@
       <c r="A23" s="3">
         <v>20</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="10"/>
+        <v>12.25</v>
+      </c>
+      <c r="D23" s="11">
+        <v>1</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0.75</v>
+      </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -1456,12 +1670,16 @@
       <c r="A24" s="3">
         <v>21</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1</v>
+      </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -1482,13 +1700,19 @@
       <c r="A25" s="3">
         <v>22</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1</v>
+      </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -1508,12 +1732,16 @@
       <c r="A26" s="3">
         <v>23</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D26" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -1534,12 +1762,16 @@
       <c r="A27" s="3">
         <v>24</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1</v>
+      </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -1560,12 +1792,16 @@
       <c r="A28" s="3">
         <v>25</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="C28" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D28" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -1586,13 +1822,19 @@
       <c r="A29" s="3">
         <v>26</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="C29" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="10"/>
+        <v>12.25</v>
+      </c>
+      <c r="D29" s="11">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0.75</v>
+      </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -1612,13 +1854,19 @@
       <c r="A30" s="3">
         <v>27</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="C30" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1</v>
+      </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -1638,12 +1886,16 @@
       <c r="A31" s="3">
         <v>28</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C31" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D31" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D31" s="10">
+        <v>1</v>
+      </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -1664,13 +1916,19 @@
       <c r="A32" s="3">
         <v>29</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="C32" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1</v>
+      </c>
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -1690,12 +1948,16 @@
       <c r="A33" s="3">
         <v>30</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="C33" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D33" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D33" s="10">
+        <v>1</v>
+      </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -1716,13 +1978,19 @@
       <c r="A34" s="3">
         <v>31</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="C34" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1</v>
+      </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -1742,13 +2010,19 @@
       <c r="A35" s="3">
         <v>32</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="C35" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -1768,12 +2042,16 @@
       <c r="A36" s="3">
         <v>33</v>
       </c>
-      <c r="B36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="C36" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D36" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -1794,13 +2072,19 @@
       <c r="A37" s="3">
         <v>34</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="C37" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1</v>
+      </c>
+      <c r="E37" s="10">
+        <v>1</v>
+      </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
@@ -1820,12 +2104,16 @@
       <c r="A38" s="3">
         <v>35</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="C38" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D38" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -1846,13 +2134,19 @@
       <c r="A39" s="3">
         <v>36</v>
       </c>
-      <c r="B39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="C39" s="6">
         <f t="shared" ref="C39" si="1">((SUM(D39:M39)*10)*70%)+(AVERAGE(N39:O39)*30%)</f>
-        <v>0</v>
-      </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
+        <v>12.25</v>
+      </c>
+      <c r="D39" s="10">
+        <v>1</v>
+      </c>
+      <c r="E39" s="10">
+        <v>0.75</v>
+      </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>

</xml_diff>

<commit_message>
update nilai xii rpl 3
</commit_message>
<xml_diff>
--- a/XIIRPL3(✿◕‿◕✿)(✿◕‿◕✿)(✿◕‿◕✿)/DATA PRAKTIK XII RPl 3.xlsx
+++ b/XIIRPL3(✿◕‿◕✿)(✿◕‿◕✿)(✿◕‿◕✿)/DATA PRAKTIK XII RPl 3.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL3(✿◕‿◕✿)(✿◕‿◕✿)(✿◕‿◕✿)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B1038A-C633-400A-88BE-9222D92B8C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0D9D61-8234-4EBC-9D3A-83FD6F3F75EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
   <sheets>
     <sheet name="NILAI ALL" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="SOAL SESI 1" sheetId="3" r:id="rId3"/>
+    <sheet name="MIGRATEMODEL" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="SOAL SESI 1" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NILAI ALL'!$G$1:$I$38</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="189">
   <si>
     <t xml:space="preserve">Nama </t>
   </si>
@@ -357,6 +358,269 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>MIGRATION</t>
+  </si>
+  <si>
+    <t>UNTUK MEMBUAT TABLE (FIELD &amp; TYPEDATA)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BISA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> UNTUK MEMBUAT DATABASE</t>
+    </r>
+  </si>
+  <si>
+    <t>TYPEDATA</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>KARAKTER</t>
+  </si>
+  <si>
+    <t>ANGKA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANGGAL </t>
+  </si>
+  <si>
+    <t>MODEL</t>
+  </si>
+  <si>
+    <t>UNTUK MENGHUBUNGKAN ANTARA DATA DI TABLE DB</t>
+  </si>
+  <si>
+    <t>DENGAN CONTROLLER</t>
+  </si>
+  <si>
+    <t>1 MODEL UNTUK 1 TABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APACHE </t>
+  </si>
+  <si>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYSQL </t>
+  </si>
+  <si>
+    <t>XAMPP</t>
+  </si>
+  <si>
+    <t>KODE BASIC</t>
+  </si>
+  <si>
+    <t>php artisan make:migration create_namatable's'_table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example </t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>php artisan make:migration create_siswas_table</t>
+  </si>
+  <si>
+    <t>php artisan make:migration create_kelass_table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lokasi file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">: </t>
+  </si>
+  <si>
+    <t>database - migration</t>
+  </si>
+  <si>
+    <t>cara eksekusi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migration </t>
+  </si>
+  <si>
+    <t>php artisan migrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cara menghapus table dan migrations </t>
+  </si>
+  <si>
+    <t>php artisan migrate:rollback</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>urutan terhapus</t>
+  </si>
+  <si>
+    <t>typedata</t>
+  </si>
+  <si>
+    <t>mysql</t>
+  </si>
+  <si>
+    <t>laravel</t>
+  </si>
+  <si>
+    <t>nama</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>mukidi</t>
+  </si>
+  <si>
+    <t>laki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slogohimo </t>
+  </si>
+  <si>
+    <t>pk 1</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>bigInt</t>
+  </si>
+  <si>
+    <t>id()</t>
+  </si>
+  <si>
+    <t>namaKelas</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>string('namaKelas')</t>
+  </si>
+  <si>
+    <t>jurusan</t>
+  </si>
+  <si>
+    <t>string('jurusan')</t>
+  </si>
+  <si>
+    <t>jumlahKursi</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>integer('jumlahKursi')</t>
+  </si>
+  <si>
+    <t>tanggalKelasDibuat</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date('tanggalKelasDibuat')</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>create_at</t>
+  </si>
+  <si>
+    <t>update_at</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>sooooal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nama field </t>
+  </si>
+  <si>
+    <t>golongandarah</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>golonganDarah</t>
+  </si>
+  <si>
+    <t>tanggaltest</t>
+  </si>
+  <si>
+    <t>berminat_donor</t>
+  </si>
+  <si>
+    <t>jumlah_donor_darah</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>penduduk</t>
+  </si>
+  <si>
+    <t>nama _bapak_kandung</t>
+  </si>
+  <si>
+    <t>nama_ibu_tiri</t>
+  </si>
+  <si>
+    <t>nama_gadis_ibu_kandung</t>
+  </si>
+  <si>
+    <t>jumlah_anak_dari_bapak</t>
   </si>
 </sst>
 </file>
@@ -366,7 +630,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot;%&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +698,14 @@
     </font>
     <font>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -826,7 +1098,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -929,6 +1201,51 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -977,45 +1294,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1040,15 +1318,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7128,7 +7406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7138,10 +7416,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
   <dimension ref="B1:AA1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F25" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="topRight" activeCell="P7" sqref="P7"/>
+      <selection pane="topRight" activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
@@ -7163,75 +7441,75 @@
     <col min="23" max="23" width="12.42578125" customWidth="1"/>
     <col min="24" max="24" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.28515625" style="73" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.28515625" style="36" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="52" t="s">
         <v>69</v>
       </c>
       <c r="D1" s="21"/>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="41" t="s">
+      <c r="F1" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="46" t="s">
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="51" t="s">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="T1" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="61" t="s">
+      <c r="U1" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="V1" s="61" t="s">
+      <c r="V1" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="W1" s="44" t="s">
+      <c r="W1" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="36"/>
+      <c r="Y1" s="51"/>
     </row>
     <row r="2" spans="2:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="64"/>
-      <c r="C2" s="37"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="52"/>
       <c r="D2" s="21"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="49"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="64"/>
       <c r="J2" s="14" t="s">
         <v>71</v>
       </c>
@@ -7259,14 +7537,14 @@
       <c r="R2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="51"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="74" t="s">
+      <c r="S2" s="66"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="AA2" s="3" t="s">
@@ -7274,13 +7552,13 @@
       </c>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="64"/>
-      <c r="C3" s="37"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
       <c r="I3" s="15" t="s">
         <v>15</v>
       </c>
@@ -7295,18 +7573,18 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="12"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="44"/>
+      <c r="S3" s="66"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="59"/>
       <c r="X3" s="31" t="s">
         <v>73</v>
       </c>
       <c r="Y3" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="Z3" s="74" t="s">
+      <c r="Z3" s="3" t="s">
         <v>77</v>
       </c>
       <c r="AA3" s="3" t="s">
@@ -7327,7 +7605,7 @@
       </c>
       <c r="H4" s="6">
         <f t="shared" ref="H4:H39" si="0">((SUM(I4:R4)*10)*70%)+(AVERAGE(T4:W4)*30%)</f>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
@@ -7342,7 +7620,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="9">
         <v>0</v>
@@ -7379,7 +7657,7 @@
       <c r="Y4" s="3">
         <v>0</v>
       </c>
-      <c r="Z4" s="74" t="s">
+      <c r="Z4" s="3" t="s">
         <v>78</v>
       </c>
       <c r="AA4" s="3" t="s">
@@ -7400,7 +7678,7 @@
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
-        <v>36.5</v>
+        <v>43.5</v>
       </c>
       <c r="I5" s="9">
         <v>1</v>
@@ -7415,7 +7693,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="9">
         <v>0</v>
@@ -7452,7 +7730,7 @@
       <c r="Y5" s="3">
         <v>15</v>
       </c>
-      <c r="Z5" s="75" t="s">
+      <c r="Z5" s="37" t="s">
         <v>82</v>
       </c>
       <c r="AA5" s="3" t="s">
@@ -7473,7 +7751,7 @@
       </c>
       <c r="H6" s="6">
         <f t="shared" si="0"/>
-        <v>40.5</v>
+        <v>47.5</v>
       </c>
       <c r="I6" s="9">
         <v>1</v>
@@ -7488,7 +7766,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="9">
         <v>0</v>
@@ -7540,7 +7818,7 @@
       </c>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>49.3</v>
       </c>
       <c r="I7" s="9">
         <v>1</v>
@@ -7555,7 +7833,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N7" s="9">
         <v>0</v>
@@ -7607,7 +7885,7 @@
       </c>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I8" s="9">
         <v>1</v>
@@ -7622,7 +7900,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="9">
         <v>0</v>
@@ -7676,7 +7954,7 @@
       </c>
       <c r="H9" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>31.849999999999998</v>
       </c>
       <c r="I9" s="10">
         <v>1</v>
@@ -7691,7 +7969,7 @@
         <v>1</v>
       </c>
       <c r="M9" s="9">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="N9" s="9">
         <v>0</v>
@@ -7726,7 +8004,7 @@
       <c r="Y9" s="3">
         <v>0</v>
       </c>
-      <c r="Z9" s="73" t="s">
+      <c r="Z9" s="36" t="s">
         <v>107</v>
       </c>
     </row>
@@ -7744,7 +8022,7 @@
       </c>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I10" s="9">
         <v>1</v>
@@ -7759,7 +8037,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="9">
         <v>0</v>
@@ -7811,7 +8089,7 @@
       </c>
       <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>29.95</v>
+        <v>36.949999999999996</v>
       </c>
       <c r="I11" s="9">
         <v>1</v>
@@ -7826,7 +8104,7 @@
         <v>0.75</v>
       </c>
       <c r="M11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="9">
         <v>0</v>
@@ -7878,7 +8156,7 @@
       </c>
       <c r="H12" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>49.3</v>
       </c>
       <c r="I12" s="9">
         <v>1</v>
@@ -7893,7 +8171,7 @@
         <v>1</v>
       </c>
       <c r="M12" s="9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N12" s="9">
         <v>0</v>
@@ -7947,7 +8225,7 @@
       </c>
       <c r="H13" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>26.599999999999998</v>
       </c>
       <c r="I13" s="9">
         <v>1</v>
@@ -7962,7 +8240,7 @@
         <v>0.75</v>
       </c>
       <c r="M13" s="9">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="N13" s="9">
         <v>0</v>
@@ -7997,7 +8275,7 @@
       <c r="Y13" s="3">
         <v>0</v>
       </c>
-      <c r="Z13" s="73" t="s">
+      <c r="Z13" s="36" t="s">
         <v>107</v>
       </c>
     </row>
@@ -8015,7 +8293,7 @@
       </c>
       <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>25.9</v>
+        <v>30.449999999999996</v>
       </c>
       <c r="I14" s="9">
         <v>1</v>
@@ -8030,7 +8308,7 @@
         <v>0.4</v>
       </c>
       <c r="M14" s="9">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="N14" s="9">
         <v>0</v>
@@ -8082,7 +8360,7 @@
       </c>
       <c r="H15" s="6">
         <f t="shared" si="0"/>
-        <v>32.75</v>
+        <v>39.049999999999997</v>
       </c>
       <c r="I15" s="9">
         <v>1</v>
@@ -8097,7 +8375,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N15" s="9">
         <v>0</v>
@@ -8149,7 +8427,7 @@
       </c>
       <c r="H16" s="6">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>43.25</v>
       </c>
       <c r="I16" s="9">
         <v>1</v>
@@ -8164,7 +8442,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N16" s="9">
         <v>0</v>
@@ -8216,7 +8494,7 @@
       </c>
       <c r="H17" s="6">
         <f t="shared" si="0"/>
-        <v>37.5</v>
+        <v>44.5</v>
       </c>
       <c r="I17" s="9">
         <v>1</v>
@@ -8231,7 +8509,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="9">
         <v>0</v>
@@ -8283,7 +8561,7 @@
       </c>
       <c r="H18" s="6">
         <f t="shared" si="0"/>
-        <v>40.5</v>
+        <v>47.5</v>
       </c>
       <c r="I18" s="9">
         <v>1</v>
@@ -8298,7 +8576,7 @@
         <v>1</v>
       </c>
       <c r="M18" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="9">
         <v>0</v>
@@ -8352,7 +8630,7 @@
       </c>
       <c r="H19" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>33.25</v>
       </c>
       <c r="I19" s="9">
         <v>1</v>
@@ -8367,7 +8645,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="9">
         <v>0</v>
@@ -8402,7 +8680,7 @@
       <c r="Y19" s="3">
         <v>0</v>
       </c>
-      <c r="Z19" s="73" t="s">
+      <c r="Z19" s="36" t="s">
         <v>107</v>
       </c>
     </row>
@@ -8420,7 +8698,7 @@
       </c>
       <c r="H20" s="6">
         <f t="shared" si="0"/>
-        <v>31.75</v>
+        <v>37</v>
       </c>
       <c r="I20" s="10">
         <v>1</v>
@@ -8435,7 +8713,7 @@
         <v>0.75</v>
       </c>
       <c r="M20" s="9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N20" s="9">
         <v>0</v>
@@ -8487,7 +8765,7 @@
       </c>
       <c r="H21" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I21" s="9">
         <v>1</v>
@@ -8502,7 +8780,7 @@
         <v>1</v>
       </c>
       <c r="M21" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="9">
         <v>0</v>
@@ -8606,7 +8884,7 @@
       <c r="Y22" s="3">
         <v>0</v>
       </c>
-      <c r="Z22" s="73" t="s">
+      <c r="Z22" s="36" t="s">
         <v>107</v>
       </c>
     </row>
@@ -8691,7 +8969,7 @@
       </c>
       <c r="H24" s="6">
         <f t="shared" si="0"/>
-        <v>38.75</v>
+        <v>44.7</v>
       </c>
       <c r="I24" s="9">
         <v>1</v>
@@ -8706,7 +8984,7 @@
         <v>0.75</v>
       </c>
       <c r="M24" s="9">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="N24" s="9">
         <v>0</v>
@@ -8758,7 +9036,7 @@
       </c>
       <c r="H25" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>49.3</v>
       </c>
       <c r="I25" s="9">
         <v>1</v>
@@ -8773,7 +9051,7 @@
         <v>1</v>
       </c>
       <c r="M25" s="9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N25" s="9">
         <v>0</v>
@@ -8825,7 +9103,7 @@
       </c>
       <c r="H26" s="6">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>37.25</v>
       </c>
       <c r="I26" s="9">
         <v>1</v>
@@ -8840,7 +9118,7 @@
         <v>1</v>
       </c>
       <c r="M26" s="9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N26" s="9">
         <v>0</v>
@@ -8958,7 +9236,7 @@
       </c>
       <c r="H28" s="6">
         <f t="shared" si="0"/>
-        <v>32.75</v>
+        <v>39.75</v>
       </c>
       <c r="I28" s="9">
         <v>1</v>
@@ -8973,7 +9251,7 @@
         <v>1</v>
       </c>
       <c r="M28" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="9">
         <v>0</v>
@@ -9025,7 +9303,7 @@
       </c>
       <c r="H29" s="6">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I29" s="10">
         <v>1</v>
@@ -9040,7 +9318,7 @@
         <v>0.75</v>
       </c>
       <c r="M29" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="9">
         <v>0</v>
@@ -9092,7 +9370,7 @@
       </c>
       <c r="H30" s="6">
         <f t="shared" si="0"/>
-        <v>41.5</v>
+        <v>48.5</v>
       </c>
       <c r="I30" s="9">
         <v>1</v>
@@ -9107,7 +9385,7 @@
         <v>1</v>
       </c>
       <c r="M30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" s="9">
         <v>0</v>
@@ -9159,7 +9437,7 @@
       </c>
       <c r="H31" s="6">
         <f t="shared" si="0"/>
-        <v>36.5</v>
+        <v>41.75</v>
       </c>
       <c r="I31" s="9">
         <v>1</v>
@@ -9174,7 +9452,7 @@
         <v>0.75</v>
       </c>
       <c r="M31" s="9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N31" s="9">
         <v>0</v>
@@ -9226,7 +9504,7 @@
       </c>
       <c r="H32" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I32" s="9">
         <v>1</v>
@@ -9241,7 +9519,7 @@
         <v>1</v>
       </c>
       <c r="M32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32" s="9">
         <v>0</v>
@@ -9295,7 +9573,7 @@
       </c>
       <c r="H33" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>26.25</v>
       </c>
       <c r="I33" s="9">
         <v>1</v>
@@ -9310,7 +9588,7 @@
         <v>0.5</v>
       </c>
       <c r="M33" s="9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N33" s="9">
         <v>0</v>
@@ -9345,7 +9623,7 @@
       <c r="Y33" s="3">
         <v>0</v>
       </c>
-      <c r="Z33" s="73" t="s">
+      <c r="Z33" s="36" t="s">
         <v>107</v>
       </c>
     </row>
@@ -9363,7 +9641,7 @@
       </c>
       <c r="H34" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I34" s="9">
         <v>1</v>
@@ -9378,7 +9656,7 @@
         <v>1</v>
       </c>
       <c r="M34" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34" s="9">
         <v>0</v>
@@ -9430,7 +9708,7 @@
       </c>
       <c r="H35" s="6">
         <f t="shared" si="0"/>
-        <v>41.8</v>
+        <v>47.05</v>
       </c>
       <c r="I35" s="9">
         <v>1</v>
@@ -9445,7 +9723,7 @@
         <v>1</v>
       </c>
       <c r="M35" s="9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N35" s="9">
         <v>0</v>
@@ -9497,7 +9775,7 @@
       </c>
       <c r="H36" s="6">
         <f t="shared" si="0"/>
-        <v>32.75</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I36" s="9">
         <v>1</v>
@@ -9512,7 +9790,7 @@
         <v>1</v>
       </c>
       <c r="M36" s="9">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="N36" s="9">
         <v>0</v>
@@ -9564,7 +9842,7 @@
       </c>
       <c r="H37" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I37" s="9">
         <v>1</v>
@@ -9579,7 +9857,7 @@
         <v>1</v>
       </c>
       <c r="M37" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -9700,7 +9978,7 @@
       </c>
       <c r="H39" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>32.549999999999997</v>
       </c>
       <c r="I39" s="9">
         <v>1</v>
@@ -9715,7 +9993,7 @@
         <v>1</v>
       </c>
       <c r="M39" s="9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N39" s="9">
         <v>0</v>
@@ -9750,7 +10028,7 @@
       <c r="Y39" s="3">
         <v>0</v>
       </c>
-      <c r="Z39" s="73" t="s">
+      <c r="Z39" s="36" t="s">
         <v>107</v>
       </c>
     </row>
@@ -9773,7 +10051,7 @@
       </c>
       <c r="M40" s="20">
         <f t="shared" ref="M40" si="3">(AVERAGE(M4:M39)*100)</f>
-        <v>0</v>
+        <v>79.861111111111114</v>
       </c>
       <c r="N40" s="20">
         <f t="shared" ref="N40" si="4">(AVERAGE(N4:N39)*100)</f>
@@ -9820,7 +10098,7 @@
       <c r="L41" s="25"/>
       <c r="M41" s="23">
         <f>AVERAGE(M40:R40)</f>
-        <v>0</v>
+        <v>13.310185185185185</v>
       </c>
       <c r="N41" s="24"/>
       <c r="O41" s="24"/>
@@ -9835,40 +10113,35 @@
     </row>
     <row r="43" spans="3:26" ht="32.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="G44" s="52" t="s">
+      <c r="G44" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="H44" s="55">
+      <c r="H44" s="41">
         <f>AVERAGE(I41,M41,T40,W40)</f>
-        <v>39.565972222222229</v>
-      </c>
-      <c r="I44" s="56"/>
+        <v>42.893518518518519</v>
+      </c>
+      <c r="I44" s="42"/>
     </row>
     <row r="45" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="G45" s="53"/>
-      <c r="H45" s="57"/>
-      <c r="I45" s="58"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="44"/>
     </row>
     <row r="46" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="G46" s="53"/>
-      <c r="H46" s="57"/>
-      <c r="I46" s="58"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="44"/>
     </row>
     <row r="47" spans="3:26" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G47" s="54"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="60"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="46"/>
     </row>
     <row r="1048576" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I1048576" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G44:G47"/>
-    <mergeCell ref="H44:I47"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="V1:V3"/>
     <mergeCell ref="X1:Y2"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="F1:F3"/>
@@ -9881,6 +10154,11 @@
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="S1:S3"/>
+    <mergeCell ref="G44:G47"/>
+    <mergeCell ref="H44:I47"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="V1:V3"/>
   </mergeCells>
   <conditionalFormatting sqref="U4:U39">
     <cfRule type="expression" dxfId="0" priority="6">
@@ -11393,6 +11671,574 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74E189E-FE33-4254-81B3-A004CD14B3D5}">
+  <dimension ref="D12:J81"/>
+  <sheetViews>
+    <sheetView topLeftCell="D72" zoomScale="390" zoomScaleNormal="390" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="G14" s="75"/>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="76" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="76"/>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="J16" s="77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I17" s="77" t="s">
+        <v>124</v>
+      </c>
+      <c r="J17" s="77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="78" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" t="s">
+        <v>129</v>
+      </c>
+      <c r="F28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="78" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F36" s="78" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="75" t="s">
+        <v>142</v>
+      </c>
+      <c r="H41" s="75"/>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>146</v>
+      </c>
+      <c r="G42" t="s">
+        <v>143</v>
+      </c>
+      <c r="H42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" t="s">
+        <v>147</v>
+      </c>
+      <c r="G43" t="s">
+        <v>154</v>
+      </c>
+      <c r="H43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>156</v>
+      </c>
+      <c r="G44" t="s">
+        <v>157</v>
+      </c>
+      <c r="H44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>159</v>
+      </c>
+      <c r="G45" t="s">
+        <v>157</v>
+      </c>
+      <c r="H45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>161</v>
+      </c>
+      <c r="G46" t="s">
+        <v>162</v>
+      </c>
+      <c r="H46" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>164</v>
+      </c>
+      <c r="G47" t="s">
+        <v>165</v>
+      </c>
+      <c r="H47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" t="s">
+        <v>169</v>
+      </c>
+      <c r="G48" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>172</v>
+      </c>
+      <c r="F49" t="s">
+        <v>170</v>
+      </c>
+      <c r="G49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>151</v>
+      </c>
+      <c r="F50" t="s">
+        <v>148</v>
+      </c>
+      <c r="G50" t="s">
+        <v>149</v>
+      </c>
+      <c r="H50" t="s">
+        <v>150</v>
+      </c>
+      <c r="I50" t="s">
+        <v>107</v>
+      </c>
+      <c r="J50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D51" s="79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D52" s="79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="61" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>174</v>
+      </c>
+      <c r="E61" t="s">
+        <v>129</v>
+      </c>
+      <c r="F61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G61" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="63" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>175</v>
+      </c>
+      <c r="G63" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>178</v>
+      </c>
+      <c r="E64" t="s">
+        <v>153</v>
+      </c>
+      <c r="F64" t="s">
+        <v>147</v>
+      </c>
+      <c r="G64" t="s">
+        <v>154</v>
+      </c>
+      <c r="H64" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="65" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>179</v>
+      </c>
+      <c r="G65" t="s">
+        <v>157</v>
+      </c>
+      <c r="H65" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="66" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>180</v>
+      </c>
+      <c r="G66" t="s">
+        <v>165</v>
+      </c>
+      <c r="H66" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="67" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>181</v>
+      </c>
+      <c r="G67" t="s">
+        <v>157</v>
+      </c>
+      <c r="H67" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>182</v>
+      </c>
+      <c r="G68" t="s">
+        <v>183</v>
+      </c>
+      <c r="H68" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="69" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>169</v>
+      </c>
+      <c r="G69" t="s">
+        <v>172</v>
+      </c>
+      <c r="H69" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>170</v>
+      </c>
+      <c r="G70" t="s">
+        <v>172</v>
+      </c>
+      <c r="H70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="72" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>174</v>
+      </c>
+      <c r="E72" t="s">
+        <v>129</v>
+      </c>
+      <c r="F72" t="s">
+        <v>184</v>
+      </c>
+      <c r="G72" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>175</v>
+      </c>
+      <c r="G74" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>178</v>
+      </c>
+      <c r="E75" t="s">
+        <v>153</v>
+      </c>
+      <c r="F75" t="s">
+        <v>147</v>
+      </c>
+      <c r="G75" t="s">
+        <v>154</v>
+      </c>
+      <c r="H75" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>185</v>
+      </c>
+      <c r="G76" t="s">
+        <v>157</v>
+      </c>
+      <c r="H76" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>186</v>
+      </c>
+      <c r="G77" t="s">
+        <v>157</v>
+      </c>
+      <c r="H77" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>187</v>
+      </c>
+      <c r="G78" t="s">
+        <v>157</v>
+      </c>
+      <c r="H78" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="79" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>188</v>
+      </c>
+      <c r="G79" t="s">
+        <v>183</v>
+      </c>
+      <c r="H79" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="80" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>169</v>
+      </c>
+      <c r="G80" t="s">
+        <v>172</v>
+      </c>
+      <c r="H80" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>170</v>
+      </c>
+      <c r="G81" t="s">
+        <v>172</v>
+      </c>
+      <c r="H81" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD728A97-A86D-4319-B892-289BC7014D66}">
   <dimension ref="E2:AI40"/>
   <sheetViews>
@@ -11410,56 +12256,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="F2" s="65">
-        <v>1</v>
-      </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65">
+      <c r="F2" s="67">
+        <v>1</v>
+      </c>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67">
         <v>2</v>
       </c>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
     </row>
     <row r="3" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E3" s="70">
-        <v>1</v>
-      </c>
-      <c r="F3" s="71" t="s">
+      <c r="E3" s="72">
+        <v>1</v>
+      </c>
+      <c r="F3" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
     </row>
     <row r="4" spans="5:35" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="E4" s="70"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
       <c r="S4" s="16" t="s">
         <v>56</v>
       </c>
@@ -11470,19 +12316,19 @@
       <c r="AI4" s="4"/>
     </row>
     <row r="5" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E5" s="70"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
       <c r="AG5" s="4">
         <v>2</v>
       </c>
@@ -11490,19 +12336,19 @@
       <c r="AI5" s="4"/>
     </row>
     <row r="6" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E6" s="70"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="74"/>
       <c r="AG6" s="4">
         <v>3</v>
       </c>
@@ -11510,19 +12356,19 @@
       <c r="AI6" s="4"/>
     </row>
     <row r="7" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E7" s="70"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
       <c r="AG7" s="4">
         <v>4</v>
       </c>
@@ -11530,23 +12376,23 @@
       <c r="AI7" s="4"/>
     </row>
     <row r="8" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E8" s="70">
+      <c r="E8" s="72">
         <v>2</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
       <c r="AG8" s="4">
         <v>5</v>
       </c>
@@ -11554,19 +12400,19 @@
       <c r="AI8" s="4"/>
     </row>
     <row r="9" spans="5:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="70"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="72"/>
-      <c r="O9" s="72"/>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
       <c r="R9" t="s">
         <v>54</v>
       </c>
@@ -11577,25 +12423,25 @@
       <c r="AI9" s="4"/>
     </row>
     <row r="10" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E10" s="70">
+      <c r="E10" s="72">
         <v>3</v>
       </c>
-      <c r="F10" s="71" t="s">
+      <c r="F10" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="71" t="s">
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="72"/>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="72"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
       <c r="U10" s="4" t="s">
         <v>57</v>
       </c>
@@ -11609,19 +12455,19 @@
       <c r="AI10" s="4"/>
     </row>
     <row r="11" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E11" s="70"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="72"/>
-      <c r="P11" s="72"/>
-      <c r="Q11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
       <c r="U11" s="4" t="s">
         <v>60</v>
       </c>
@@ -11635,19 +12481,19 @@
       <c r="AI11" s="4"/>
     </row>
     <row r="12" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E12" s="70"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="72"/>
-      <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
-      <c r="Q12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
       <c r="U12" s="4" t="s">
         <v>59</v>
       </c>
@@ -11661,19 +12507,19 @@
       <c r="AI12" s="4"/>
     </row>
     <row r="13" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E13" s="70"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="72"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="72"/>
-      <c r="O13" s="72"/>
-      <c r="P13" s="72"/>
-      <c r="Q13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
       <c r="U13" s="4" t="s">
         <v>62</v>
       </c>
@@ -11687,19 +12533,19 @@
       <c r="AI13" s="4"/>
     </row>
     <row r="14" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E14" s="70"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
-      <c r="P14" s="72"/>
-      <c r="Q14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="74"/>
+      <c r="P14" s="74"/>
+      <c r="Q14" s="74"/>
       <c r="AG14" s="4">
         <v>11</v>
       </c>
@@ -11707,262 +12553,262 @@
       <c r="AI14" s="4"/>
     </row>
     <row r="15" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E15" s="70"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="72"/>
-      <c r="O15" s="72"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="74"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="74"/>
     </row>
     <row r="16" spans="5:35" x14ac:dyDescent="0.25">
-      <c r="E16" s="70"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="74"/>
+      <c r="Q16" s="74"/>
     </row>
     <row r="17" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E17" s="70"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="74"/>
+      <c r="Q17" s="74"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="70"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="72"/>
-      <c r="O18" s="72"/>
-      <c r="P18" s="72"/>
-      <c r="Q18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="74"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
+      <c r="N18" s="74"/>
+      <c r="O18" s="74"/>
+      <c r="P18" s="74"/>
+      <c r="Q18" s="74"/>
     </row>
     <row r="19" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="70"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
-      <c r="N19" s="72"/>
-      <c r="O19" s="72"/>
-      <c r="P19" s="72"/>
-      <c r="Q19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="74"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="74"/>
+      <c r="P19" s="74"/>
+      <c r="Q19" s="74"/>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="70"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="72"/>
-      <c r="O20" s="72"/>
-      <c r="P20" s="72"/>
-      <c r="Q20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="74"/>
+      <c r="N20" s="74"/>
+      <c r="O20" s="74"/>
+      <c r="P20" s="74"/>
+      <c r="Q20" s="74"/>
     </row>
     <row r="21" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E21" s="70"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="72"/>
-      <c r="N21" s="72"/>
-      <c r="O21" s="72"/>
-      <c r="P21" s="72"/>
-      <c r="Q21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="74"/>
+      <c r="O21" s="74"/>
+      <c r="P21" s="74"/>
+      <c r="Q21" s="74"/>
     </row>
     <row r="22" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E22" s="70"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="72"/>
-      <c r="O22" s="72"/>
-      <c r="P22" s="72"/>
-      <c r="Q22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="74"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="74"/>
     </row>
     <row r="23" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="70"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
-      <c r="O23" s="72"/>
-      <c r="P23" s="72"/>
-      <c r="Q23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="74"/>
     </row>
     <row r="24" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E24" s="70"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="72"/>
-      <c r="K24" s="72"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="72"/>
-      <c r="P24" s="72"/>
-      <c r="Q24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="74"/>
+      <c r="O24" s="74"/>
+      <c r="P24" s="74"/>
+      <c r="Q24" s="74"/>
     </row>
     <row r="25" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E25" s="70"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="72"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="72"/>
-      <c r="N25" s="72"/>
-      <c r="O25" s="72"/>
-      <c r="P25" s="72"/>
-      <c r="Q25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="74"/>
+      <c r="O25" s="74"/>
+      <c r="P25" s="74"/>
+      <c r="Q25" s="74"/>
     </row>
     <row r="26" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E26" s="70"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
-      <c r="N26" s="72"/>
-      <c r="O26" s="72"/>
-      <c r="P26" s="72"/>
-      <c r="Q26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="74"/>
+      <c r="M26" s="74"/>
+      <c r="N26" s="74"/>
+      <c r="O26" s="74"/>
+      <c r="P26" s="74"/>
+      <c r="Q26" s="74"/>
     </row>
     <row r="27" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E27" s="70"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="72"/>
-      <c r="K27" s="72"/>
-      <c r="L27" s="72"/>
-      <c r="M27" s="72"/>
-      <c r="N27" s="72"/>
-      <c r="O27" s="72"/>
-      <c r="P27" s="72"/>
-      <c r="Q27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="74"/>
+      <c r="O27" s="74"/>
+      <c r="P27" s="74"/>
+      <c r="Q27" s="74"/>
     </row>
     <row r="28" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="70"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="72"/>
-      <c r="M28" s="72"/>
-      <c r="N28" s="72"/>
-      <c r="O28" s="72"/>
-      <c r="P28" s="72"/>
-      <c r="Q28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="74"/>
+      <c r="M28" s="74"/>
+      <c r="N28" s="74"/>
+      <c r="O28" s="74"/>
+      <c r="P28" s="74"/>
+      <c r="Q28" s="74"/>
     </row>
     <row r="29" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E29" s="70">
+      <c r="E29" s="72">
         <v>4</v>
       </c>
-      <c r="F29" s="71" t="s">
+      <c r="F29" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="72"/>
-      <c r="K29" s="72"/>
-      <c r="L29" s="72"/>
-      <c r="M29" s="72"/>
-      <c r="N29" s="72"/>
-      <c r="O29" s="72"/>
-      <c r="P29" s="72"/>
-      <c r="Q29" s="72"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="74"/>
+      <c r="O29" s="74"/>
+      <c r="P29" s="74"/>
+      <c r="Q29" s="74"/>
     </row>
     <row r="30" spans="5:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="70"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72"/>
-      <c r="K30" s="72"/>
-      <c r="L30" s="72"/>
-      <c r="M30" s="72"/>
-      <c r="N30" s="72"/>
-      <c r="O30" s="72"/>
-      <c r="P30" s="72"/>
-      <c r="Q30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="74"/>
+      <c r="O30" s="74"/>
+      <c r="P30" s="74"/>
+      <c r="Q30" s="74"/>
     </row>
     <row r="38" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F38" s="66" t="s">
+      <c r="F38" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="66"/>
-      <c r="H38" s="66"/>
-      <c r="I38" s="66"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="68"/>
     </row>
     <row r="39" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F39" s="66" t="s">
+      <c r="F39" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="G39" s="66"/>
+      <c r="G39" s="68"/>
       <c r="H39" s="4" t="s">
         <v>66</v>
       </c>
@@ -11971,12 +12817,12 @@
       </c>
     </row>
     <row r="40" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F40" s="67" t="s">
+      <c r="F40" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="69"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -12000,7 +12846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151E02DC-2DD5-4834-8E2C-C42882C3EBF9}">
   <dimension ref="A1:C14"/>
   <sheetViews>

</xml_diff>